<commit_message>
bergupdate: CGHcall now produces a graph that shows which probes MaxMiss removes from 1 sample.
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/Gantt.xlsx
+++ b/docs/docs_I_made/Gantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Faire les slides qui présentent chacun des 4 outils (OncoscanR, EaCoN, rCGH, CGHcall) efficacement et facilement</t>
   </si>
@@ -65,9 +65,6 @@
     <t>ecriture rapport</t>
   </si>
   <si>
-    <t>peaufiner slides, les montrer à des gens</t>
-  </si>
-  <si>
     <t>s'entrainer pour la soutenance</t>
   </si>
   <si>
@@ -75,6 +72,12 @@
   </si>
   <si>
     <t>implémenter le pipeline de routine</t>
+  </si>
+  <si>
+    <t>peaufiner slides soutenance, les montrer à des gens</t>
+  </si>
+  <si>
+    <t>fin officielle du stage</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,12 +103,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,33 +161,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -481,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EY5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN14" sqref="AN14"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2:BM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +484,7 @@
     <col min="29" max="29" width="11.42578125" style="3"/>
     <col min="30" max="30" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
@@ -960,263 +955,264 @@
       </c>
     </row>
     <row r="2" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="7"/>
-      <c r="BB2" s="5" t="s">
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
+      <c r="AY2" s="11"/>
+      <c r="BB2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5"/>
-      <c r="BL2" s="5"/>
-      <c r="BM2" s="5"/>
-      <c r="BZ2" s="13" t="s">
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="7"/>
+      <c r="BH2" s="7"/>
+      <c r="BI2" s="7"/>
+      <c r="BJ2" s="7"/>
+      <c r="BK2" s="7"/>
+      <c r="BL2" s="7"/>
+      <c r="BM2" s="7"/>
+      <c r="BZ2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="CA2" s="13"/>
-      <c r="CB2" s="13"/>
-      <c r="CC2" s="13"/>
-      <c r="CD2" s="13"/>
-      <c r="CE2" s="13"/>
-      <c r="CF2" s="13"/>
-      <c r="CG2" s="13"/>
-      <c r="CH2" s="13"/>
-      <c r="CI2" s="13"/>
-      <c r="CJ2" s="13"/>
-      <c r="CK2" s="13"/>
-      <c r="CL2" s="13"/>
-      <c r="CM2" s="13"/>
-      <c r="CN2" s="13"/>
-      <c r="CO2" s="13"/>
-      <c r="CP2" s="13"/>
-      <c r="CQ2" s="13"/>
-      <c r="CR2" s="13"/>
-      <c r="CS2" s="13"/>
-      <c r="CT2" s="13"/>
-      <c r="CU2" s="13"/>
-      <c r="CV2" s="13"/>
-      <c r="CW2" s="13"/>
-      <c r="CX2" s="13"/>
-      <c r="CY2" s="13"/>
-      <c r="DB2" s="4" t="s">
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="8"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="DB2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="DC2" s="4"/>
-      <c r="DD2" s="4"/>
-      <c r="DE2" s="4"/>
-      <c r="DF2" s="4"/>
-      <c r="DI2" s="11" t="s">
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8"/>
+      <c r="DI2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="DJ2" s="11"/>
-      <c r="DK2" s="11"/>
-      <c r="DL2" s="11"/>
-      <c r="DM2" s="11"/>
-      <c r="DP2" s="9" t="s">
+      <c r="DJ2" s="9"/>
+      <c r="DK2" s="9"/>
+      <c r="DL2" s="9"/>
+      <c r="DM2" s="9"/>
+      <c r="DP2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="DQ2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="DR2" s="13"/>
-      <c r="DS2" s="13"/>
-      <c r="DT2" s="13"/>
-      <c r="DU2" s="13"/>
-      <c r="DV2" s="13"/>
-      <c r="DW2" s="13"/>
-      <c r="DX2" s="13"/>
-      <c r="DY2" s="13"/>
-      <c r="DZ2" s="13"/>
-      <c r="EA2" s="13"/>
-      <c r="EB2" s="13"/>
-      <c r="EC2" s="13"/>
-      <c r="ED2" s="13"/>
-      <c r="EE2" s="13"/>
-      <c r="EF2" s="13"/>
-      <c r="EG2" s="13"/>
-      <c r="EH2" s="13"/>
-      <c r="EK2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="EL2" s="13"/>
-      <c r="EM2" s="13"/>
-      <c r="EN2" s="13"/>
-      <c r="EO2" s="13"/>
-      <c r="ER2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="ES2" s="13"/>
-      <c r="ET2" s="13"/>
-      <c r="EU2" s="13"/>
-      <c r="EV2" s="13"/>
-      <c r="EW2" s="10" t="s">
+      <c r="DS2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="EX2" s="10"/>
+      <c r="DT2" s="10"/>
+      <c r="EY2" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AD3" s="4" t="s">
+      <c r="AD3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="6" t="s">
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="4" t="s">
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="12"/>
+      <c r="AO3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="4"/>
-      <c r="AS3" s="4"/>
-      <c r="AT3" s="6" t="s">
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AU3" s="6"/>
-      <c r="AV3" s="6"/>
-      <c r="AW3" s="6"/>
-      <c r="AX3" s="6"/>
-      <c r="AY3" s="6"/>
-      <c r="BL3" s="4" t="s">
+      <c r="AU3" s="12"/>
+      <c r="AV3" s="12"/>
+      <c r="AW3" s="12"/>
+      <c r="AX3" s="12"/>
+      <c r="AY3" s="12"/>
+      <c r="BL3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="8"/>
+      <c r="BR3" s="8"/>
+      <c r="BS3" s="8"/>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="CC3" s="8"/>
+      <c r="CD3" s="8"/>
+      <c r="CL3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="CM3" s="7"/>
+      <c r="CN3" s="7"/>
+      <c r="CO3" s="7"/>
+      <c r="CP3" s="7"/>
+      <c r="CQ3" s="7"/>
+      <c r="CR3" s="7"/>
+      <c r="CS3" s="7"/>
+      <c r="CT3" s="7"/>
+      <c r="CU3" s="7"/>
+      <c r="CV3" s="7"/>
+      <c r="CW3" s="7"/>
+      <c r="CX3" s="7"/>
+      <c r="CY3" s="7"/>
+      <c r="CZ3" s="7"/>
+      <c r="DA3" s="7"/>
+      <c r="DB3" s="7"/>
+      <c r="DC3" s="7"/>
+      <c r="DI3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="BM3" s="4"/>
-      <c r="BN3" s="4"/>
-      <c r="BO3" s="4"/>
-      <c r="BP3" s="4"/>
-      <c r="BQ3" s="4"/>
-      <c r="BR3" s="4"/>
-      <c r="BS3" s="4"/>
-      <c r="BT3" s="4"/>
-      <c r="BU3" s="4"/>
-      <c r="BV3" s="4"/>
-      <c r="BW3" s="4"/>
-      <c r="BX3" s="4"/>
-      <c r="BY3" s="4"/>
-      <c r="BZ3" s="4"/>
-      <c r="CA3" s="4"/>
-      <c r="CB3" s="4"/>
-      <c r="CC3" s="4"/>
-      <c r="CD3" s="4"/>
+      <c r="DJ3" s="7"/>
+      <c r="DK3" s="7"/>
+      <c r="DL3" s="7"/>
+      <c r="DM3" s="7"/>
+      <c r="DP3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="DQ3" s="7"/>
+      <c r="DR3" s="7"/>
     </row>
     <row r="4" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AD4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX4" s="11" t="s">
+      <c r="AD4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AY4" s="11"/>
-      <c r="AZ4" s="11"/>
-      <c r="BA4" s="11"/>
-      <c r="BB4" s="11"/>
+      <c r="AY4" s="9"/>
+      <c r="AZ4" s="9"/>
+      <c r="BA4" s="9"/>
+      <c r="BB4" s="9"/>
     </row>
     <row r="5" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AY5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="BF5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="BM5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="BT5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="CA5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="CH5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="CO5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="CV5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="DC5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="DJ5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="DQ5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="DX5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="EE5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="EL5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="ES5" s="12" t="s">
+      <c r="AY5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BT5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="CA5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="CH5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="CO5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="CV5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="DC5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="DJ5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="DQ5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="DX5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="EE5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="EL5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="ES5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="DQ2:EH2"/>
+    <mergeCell ref="CL3:DC3"/>
     <mergeCell ref="BL3:CD3"/>
     <mergeCell ref="AX4:BB4"/>
     <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="EW2:EX2"/>
+    <mergeCell ref="DS2:DT2"/>
     <mergeCell ref="BB2:BM2"/>
     <mergeCell ref="DB2:DF2"/>
     <mergeCell ref="DI2:DM2"/>
     <mergeCell ref="BZ2:CY2"/>
-    <mergeCell ref="EK2:EO2"/>
-    <mergeCell ref="ER2:EV2"/>
+    <mergeCell ref="DI3:DM3"/>
     <mergeCell ref="AD2:AY2"/>
     <mergeCell ref="AI3:AN3"/>
     <mergeCell ref="AO3:AS3"/>
     <mergeCell ref="AT3:AY3"/>
+    <mergeCell ref="DP3:DR3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bergupdate : added notes on ASCAT
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/Gantt.xlsx
+++ b/docs/docs_I_made/Gantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Faire les slides qui présentent chacun des 4 outils (OncoscanR, EaCoN, rCGH, CGHcall) efficacement et facilement</t>
   </si>
@@ -53,9 +53,6 @@
     <t>réunion suivi</t>
   </si>
   <si>
-    <t>Calculer le Gi sur tous échantillons (Oncoscan et Agilent) sur les 4 outils</t>
-  </si>
-  <si>
     <t>peaufiner et envoyer le rapport à plusieurs personnes</t>
   </si>
   <si>
@@ -71,13 +68,34 @@
     <t>préparer la soutenance</t>
   </si>
   <si>
-    <t>implémenter le pipeline de routine</t>
-  </si>
-  <si>
     <t>peaufiner slides soutenance, les montrer à des gens</t>
   </si>
   <si>
     <t>fin officielle du stage</t>
+  </si>
+  <si>
+    <t>formation CHAS</t>
+  </si>
+  <si>
+    <t>rapport fini</t>
+  </si>
+  <si>
+    <t>choix package</t>
+  </si>
+  <si>
+    <t>approfondir sur la comparaison des outils</t>
+  </si>
+  <si>
+    <t>calculer GI pour tous outils</t>
+  </si>
+  <si>
+    <t>dernières touches sur le rapport</t>
+  </si>
+  <si>
+    <t>envoyer plan détaillé du rapport à slim karkar</t>
+  </si>
+  <si>
+    <t>envoyer plan détaillé du rapport à slim karkar - dernier délai</t>
   </si>
 </sst>
 </file>
@@ -93,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +166,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -169,6 +199,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -185,6 +219,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EY5"/>
+  <dimension ref="A1:EY7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2:BM2"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CJ19" sqref="CJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,181 +992,178 @@
       </c>
     </row>
     <row r="2" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AD2" s="11" t="s">
+      <c r="AD2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="11"/>
-      <c r="AV2" s="11"/>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11"/>
-      <c r="AY2" s="11"/>
-      <c r="BB2" s="7" t="s">
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
+      <c r="AP2" s="13"/>
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="13"/>
+      <c r="AS2" s="13"/>
+      <c r="AT2" s="13"/>
+      <c r="AU2" s="13"/>
+      <c r="AV2" s="13"/>
+      <c r="AW2" s="13"/>
+      <c r="AX2" s="13"/>
+      <c r="AY2" s="13"/>
+      <c r="BB2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+      <c r="BK2" s="9"/>
+      <c r="BL2" s="9"/>
+      <c r="BM2" s="9"/>
+      <c r="BZ2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10"/>
+      <c r="CC2" s="10"/>
+      <c r="CD2" s="10"/>
+      <c r="CG2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="CH2" s="10"/>
+      <c r="CI2" s="10"/>
+      <c r="CJ2" s="10"/>
+      <c r="CK2" s="10"/>
+      <c r="CN2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="BC2" s="7"/>
-      <c r="BD2" s="7"/>
-      <c r="BE2" s="7"/>
-      <c r="BF2" s="7"/>
-      <c r="BG2" s="7"/>
-      <c r="BH2" s="7"/>
-      <c r="BI2" s="7"/>
-      <c r="BJ2" s="7"/>
-      <c r="BK2" s="7"/>
-      <c r="BL2" s="7"/>
-      <c r="BM2" s="7"/>
-      <c r="BZ2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="CA2" s="8"/>
-      <c r="CB2" s="8"/>
-      <c r="CC2" s="8"/>
-      <c r="CD2" s="8"/>
-      <c r="CE2" s="8"/>
-      <c r="CF2" s="8"/>
-      <c r="CG2" s="8"/>
-      <c r="CH2" s="8"/>
-      <c r="CI2" s="8"/>
-      <c r="CJ2" s="8"/>
-      <c r="CK2" s="8"/>
-      <c r="CL2" s="8"/>
-      <c r="CM2" s="8"/>
-      <c r="CN2" s="8"/>
-      <c r="CO2" s="8"/>
-      <c r="CP2" s="8"/>
-      <c r="CQ2" s="8"/>
-      <c r="CR2" s="8"/>
-      <c r="CS2" s="8"/>
-      <c r="CT2" s="8"/>
-      <c r="CU2" s="8"/>
-      <c r="CV2" s="8"/>
-      <c r="CW2" s="8"/>
-      <c r="CX2" s="8"/>
-      <c r="CY2" s="8"/>
-      <c r="DB2" s="8" t="s">
+      <c r="CO2" s="10"/>
+      <c r="CP2" s="10"/>
+      <c r="CQ2" s="10"/>
+      <c r="CR2" s="10"/>
+      <c r="CS2" s="10"/>
+      <c r="CT2" s="10"/>
+      <c r="CU2" s="10"/>
+      <c r="CV2" s="10"/>
+      <c r="CW2" s="10"/>
+      <c r="CX2" s="10"/>
+      <c r="CY2" s="10"/>
+      <c r="DB2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="DC2" s="10"/>
+      <c r="DD2" s="10"/>
+      <c r="DE2" s="10"/>
+      <c r="DF2" s="10"/>
+      <c r="DI2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="DC2" s="8"/>
-      <c r="DD2" s="8"/>
-      <c r="DE2" s="8"/>
-      <c r="DF2" s="8"/>
-      <c r="DI2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="DJ2" s="9"/>
-      <c r="DK2" s="9"/>
-      <c r="DL2" s="9"/>
-      <c r="DM2" s="9"/>
+      <c r="DJ2" s="11"/>
+      <c r="DK2" s="11"/>
+      <c r="DL2" s="11"/>
+      <c r="DM2" s="11"/>
       <c r="DP2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="DS2" s="10" t="s">
+      <c r="DS2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="DT2" s="10"/>
+      <c r="DT2" s="12"/>
       <c r="EY2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AD3" s="8" t="s">
+      <c r="AD3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
       <c r="AH3" s="4"/>
-      <c r="AI3" s="12" t="s">
+      <c r="AI3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="8" t="s">
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="12" t="s">
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AU3" s="12"/>
-      <c r="AV3" s="12"/>
-      <c r="AW3" s="12"/>
-      <c r="AX3" s="12"/>
-      <c r="AY3" s="12"/>
-      <c r="BL3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="8"/>
-      <c r="BR3" s="8"/>
-      <c r="BS3" s="8"/>
-      <c r="BT3" s="8"/>
-      <c r="BU3" s="8"/>
-      <c r="BV3" s="8"/>
-      <c r="BW3" s="8"/>
-      <c r="BX3" s="8"/>
-      <c r="BY3" s="8"/>
-      <c r="BZ3" s="8"/>
-      <c r="CA3" s="8"/>
-      <c r="CB3" s="8"/>
-      <c r="CC3" s="8"/>
-      <c r="CD3" s="8"/>
-      <c r="CL3" s="7" t="s">
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="14"/>
+      <c r="AX3" s="14"/>
+      <c r="AY3" s="14"/>
+      <c r="BA3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB3" s="15"/>
+      <c r="BL3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="BM3" s="10"/>
+      <c r="BN3" s="10"/>
+      <c r="BO3" s="10"/>
+      <c r="BP3" s="10"/>
+      <c r="BS3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="BT3" s="10"/>
+      <c r="BU3" s="10"/>
+      <c r="BV3" s="10"/>
+      <c r="BW3" s="10"/>
+      <c r="CL3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="CM3" s="9"/>
+      <c r="CN3" s="9"/>
+      <c r="CO3" s="9"/>
+      <c r="CP3" s="9"/>
+      <c r="CQ3" s="9"/>
+      <c r="CR3" s="9"/>
+      <c r="CS3" s="9"/>
+      <c r="CT3" s="9"/>
+      <c r="CU3" s="9"/>
+      <c r="CV3" s="9"/>
+      <c r="CW3" s="9"/>
+      <c r="CX3" s="9"/>
+      <c r="CY3" s="9"/>
+      <c r="CZ3" s="9"/>
+      <c r="DA3" s="9"/>
+      <c r="DB3" s="9"/>
+      <c r="DC3" s="9"/>
+      <c r="DI3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="CM3" s="7"/>
-      <c r="CN3" s="7"/>
-      <c r="CO3" s="7"/>
-      <c r="CP3" s="7"/>
-      <c r="CQ3" s="7"/>
-      <c r="CR3" s="7"/>
-      <c r="CS3" s="7"/>
-      <c r="CT3" s="7"/>
-      <c r="CU3" s="7"/>
-      <c r="CV3" s="7"/>
-      <c r="CW3" s="7"/>
-      <c r="CX3" s="7"/>
-      <c r="CY3" s="7"/>
-      <c r="CZ3" s="7"/>
-      <c r="DA3" s="7"/>
-      <c r="DB3" s="7"/>
-      <c r="DC3" s="7"/>
-      <c r="DI3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="DJ3" s="7"/>
-      <c r="DK3" s="7"/>
-      <c r="DL3" s="7"/>
-      <c r="DM3" s="7"/>
-      <c r="DP3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="DQ3" s="7"/>
-      <c r="DR3" s="7"/>
+      <c r="DJ3" s="9"/>
+      <c r="DK3" s="9"/>
+      <c r="DL3" s="9"/>
+      <c r="DM3" s="9"/>
+      <c r="DP3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="DQ3" s="9"/>
+      <c r="DR3" s="9"/>
     </row>
     <row r="4" spans="1:155" x14ac:dyDescent="0.25">
       <c r="AD4" s="6" t="s">
@@ -1141,13 +1175,13 @@
       <c r="AR4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AX4" s="9" t="s">
+      <c r="AX4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AY4" s="9"/>
-      <c r="AZ4" s="9"/>
-      <c r="BA4" s="9"/>
-      <c r="BB4" s="9"/>
+      <c r="AY4" s="11"/>
+      <c r="AZ4" s="11"/>
+      <c r="BA4" s="11"/>
+      <c r="BB4" s="11"/>
     </row>
     <row r="5" spans="1:155" x14ac:dyDescent="0.25">
       <c r="AY5" s="6" t="s">
@@ -1196,23 +1230,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="CG6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="CK6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="BS7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="BT7" s="8"/>
+      <c r="BU7" s="8"/>
+      <c r="BV7" s="8"/>
+      <c r="BW7" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="CL3:DC3"/>
-    <mergeCell ref="BL3:CD3"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="DS2:DT2"/>
-    <mergeCell ref="BB2:BM2"/>
+  <mergeCells count="20">
+    <mergeCell ref="DP3:DR3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="CN2:CY2"/>
     <mergeCell ref="DB2:DF2"/>
-    <mergeCell ref="DI2:DM2"/>
-    <mergeCell ref="BZ2:CY2"/>
+    <mergeCell ref="BZ2:CD2"/>
+    <mergeCell ref="CG2:CK2"/>
+    <mergeCell ref="BS3:BW3"/>
     <mergeCell ref="DI3:DM3"/>
     <mergeCell ref="AD2:AY2"/>
     <mergeCell ref="AI3:AN3"/>
     <mergeCell ref="AO3:AS3"/>
     <mergeCell ref="AT3:AY3"/>
-    <mergeCell ref="DP3:DR3"/>
+    <mergeCell ref="DS2:DT2"/>
+    <mergeCell ref="BB2:BM2"/>
+    <mergeCell ref="DI2:DM2"/>
+    <mergeCell ref="BS7:BW7"/>
+    <mergeCell ref="CL3:DC3"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="BL3:BP3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bergupdate: changed comparative table, and things in scripts also.
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/Gantt.xlsx
+++ b/docs/docs_I_made/Gantt.xlsx
@@ -200,19 +200,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -221,7 +215,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EY7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CJ19" sqref="CJ19"/>
+    <sheetView tabSelected="1" topLeftCell="BO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CC22" sqref="CC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,44 +992,44 @@
       </c>
     </row>
     <row r="2" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="AD2" s="13" t="s">
+      <c r="AD2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="13"/>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="13"/>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13"/>
-      <c r="AQ2" s="13"/>
-      <c r="AR2" s="13"/>
-      <c r="AS2" s="13"/>
-      <c r="AT2" s="13"/>
-      <c r="AU2" s="13"/>
-      <c r="AV2" s="13"/>
-      <c r="AW2" s="13"/>
-      <c r="AX2" s="13"/>
-      <c r="AY2" s="13"/>
-      <c r="BB2" s="9" t="s">
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
+      <c r="AY2" s="11"/>
+      <c r="BB2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
       <c r="BZ2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1065,20 +1065,20 @@
       <c r="DD2" s="10"/>
       <c r="DE2" s="10"/>
       <c r="DF2" s="10"/>
-      <c r="DI2" s="11" t="s">
+      <c r="DI2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="DJ2" s="11"/>
-      <c r="DK2" s="11"/>
-      <c r="DL2" s="11"/>
-      <c r="DM2" s="11"/>
+      <c r="DJ2" s="14"/>
+      <c r="DK2" s="14"/>
+      <c r="DL2" s="14"/>
+      <c r="DM2" s="14"/>
       <c r="DP2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="DS2" s="12" t="s">
+      <c r="DS2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="DT2" s="12"/>
+      <c r="DT2" s="13"/>
       <c r="EY2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1091,14 +1091,14 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="4"/>
-      <c r="AI3" s="14" t="s">
+      <c r="AI3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
-      <c r="AM3" s="14"/>
-      <c r="AN3" s="14"/>
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="12"/>
       <c r="AO3" s="10" t="s">
         <v>3</v>
       </c>
@@ -1106,18 +1106,18 @@
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
       <c r="AS3" s="10"/>
-      <c r="AT3" s="14" t="s">
+      <c r="AT3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AU3" s="14"/>
-      <c r="AV3" s="14"/>
-      <c r="AW3" s="14"/>
-      <c r="AX3" s="14"/>
-      <c r="AY3" s="14"/>
-      <c r="BA3" s="15" t="s">
+      <c r="AU3" s="12"/>
+      <c r="AV3" s="12"/>
+      <c r="AW3" s="12"/>
+      <c r="AX3" s="12"/>
+      <c r="AY3" s="12"/>
+      <c r="BA3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="BB3" s="15"/>
+      <c r="BB3" s="9"/>
       <c r="BL3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1132,38 +1132,38 @@
       <c r="BU3" s="10"/>
       <c r="BV3" s="10"/>
       <c r="BW3" s="10"/>
-      <c r="CL3" s="9" t="s">
+      <c r="CL3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="CM3" s="9"/>
-      <c r="CN3" s="9"/>
-      <c r="CO3" s="9"/>
-      <c r="CP3" s="9"/>
-      <c r="CQ3" s="9"/>
-      <c r="CR3" s="9"/>
-      <c r="CS3" s="9"/>
-      <c r="CT3" s="9"/>
-      <c r="CU3" s="9"/>
-      <c r="CV3" s="9"/>
-      <c r="CW3" s="9"/>
-      <c r="CX3" s="9"/>
-      <c r="CY3" s="9"/>
-      <c r="CZ3" s="9"/>
-      <c r="DA3" s="9"/>
-      <c r="DB3" s="9"/>
-      <c r="DC3" s="9"/>
-      <c r="DI3" s="9" t="s">
+      <c r="CM3" s="8"/>
+      <c r="CN3" s="8"/>
+      <c r="CO3" s="8"/>
+      <c r="CP3" s="8"/>
+      <c r="CQ3" s="8"/>
+      <c r="CR3" s="8"/>
+      <c r="CS3" s="8"/>
+      <c r="CT3" s="8"/>
+      <c r="CU3" s="8"/>
+      <c r="CV3" s="8"/>
+      <c r="CW3" s="8"/>
+      <c r="CX3" s="8"/>
+      <c r="CY3" s="8"/>
+      <c r="CZ3" s="8"/>
+      <c r="DA3" s="8"/>
+      <c r="DB3" s="8"/>
+      <c r="DC3" s="8"/>
+      <c r="DI3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="DJ3" s="9"/>
-      <c r="DK3" s="9"/>
-      <c r="DL3" s="9"/>
-      <c r="DM3" s="9"/>
-      <c r="DP3" s="9" t="s">
+      <c r="DJ3" s="8"/>
+      <c r="DK3" s="8"/>
+      <c r="DL3" s="8"/>
+      <c r="DM3" s="8"/>
+      <c r="DP3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="DQ3" s="9"/>
-      <c r="DR3" s="9"/>
+      <c r="DQ3" s="8"/>
+      <c r="DR3" s="8"/>
     </row>
     <row r="4" spans="1:155" x14ac:dyDescent="0.25">
       <c r="AD4" s="6" t="s">
@@ -1175,13 +1175,13 @@
       <c r="AR4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AX4" s="11" t="s">
+      <c r="AX4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="AY4" s="11"/>
-      <c r="AZ4" s="11"/>
-      <c r="BA4" s="11"/>
-      <c r="BB4" s="11"/>
+      <c r="AY4" s="14"/>
+      <c r="AZ4" s="14"/>
+      <c r="BA4" s="14"/>
+      <c r="BB4" s="14"/>
     </row>
     <row r="5" spans="1:155" x14ac:dyDescent="0.25">
       <c r="AY5" s="6" t="s">
@@ -1242,16 +1242,28 @@
       </c>
     </row>
     <row r="7" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="BS7" s="8" t="s">
+      <c r="BS7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="BT7" s="8"/>
-      <c r="BU7" s="8"/>
-      <c r="BV7" s="8"/>
-      <c r="BW7" s="8"/>
+      <c r="BT7" s="15"/>
+      <c r="BU7" s="15"/>
+      <c r="BV7" s="15"/>
+      <c r="BW7" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="BS7:BW7"/>
+    <mergeCell ref="CL3:DC3"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="AD2:AY2"/>
+    <mergeCell ref="AI3:AN3"/>
+    <mergeCell ref="AO3:AS3"/>
+    <mergeCell ref="AT3:AY3"/>
+    <mergeCell ref="DS2:DT2"/>
+    <mergeCell ref="BB2:BM2"/>
+    <mergeCell ref="DI2:DM2"/>
     <mergeCell ref="DP3:DR3"/>
     <mergeCell ref="BA3:BB3"/>
     <mergeCell ref="CN2:CY2"/>
@@ -1260,18 +1272,6 @@
     <mergeCell ref="CG2:CK2"/>
     <mergeCell ref="BS3:BW3"/>
     <mergeCell ref="DI3:DM3"/>
-    <mergeCell ref="AD2:AY2"/>
-    <mergeCell ref="AI3:AN3"/>
-    <mergeCell ref="AO3:AS3"/>
-    <mergeCell ref="AT3:AY3"/>
-    <mergeCell ref="DS2:DT2"/>
-    <mergeCell ref="BB2:BM2"/>
-    <mergeCell ref="DI2:DM2"/>
-    <mergeCell ref="BS7:BW7"/>
-    <mergeCell ref="CL3:DC3"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="BL3:BP3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>